<commit_message>
Fixed metrics generation bug
</commit_message>
<xml_diff>
--- a/Descriptions.xlsx
+++ b/Descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean\Dropbox\NREL Work\Year 2020\NOVA\Metrics at Scale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3741CC94-92CB-4131-9794-FB684DE75644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340F32AF-4223-44A3-9613-EF866C2794D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="255" windowWidth="21795" windowHeight="13635" xr2:uid="{D2247365-3C67-4207-B7B7-8EA470B2C26E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2247365-3C67-4207-B7B7-8EA470B2C26E}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="156">
   <si>
     <t>filenames</t>
   </si>
@@ -459,14 +459,67 @@
   </si>
   <si>
     <t>Technologies (PV, Storage, HVAC, HPWH, ERWH)</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Includes relevant metrics for the cost effectiveness of the system such as NPV, annual bill savings, and system upfront costs</t>
+  </si>
+  <si>
+    <t>Breaks out costs into respective components, such as utility energy costs and system CAPEX and O&amp;M costs</t>
+  </si>
+  <si>
+    <t>Metrics relevant to home performance such as annual load and home comfort</t>
+  </si>
+  <si>
+    <t>Metrics relevant to utility and other stakeholders. These include grid impacts and environmental impacts.</t>
+  </si>
+  <si>
+    <t>Metrics on system upgrades and technology performance, such as system capacity. Mainly useful for determining case</t>
+  </si>
+  <si>
+    <t>Used to identify case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute value of run, does not use baseline comparison. </t>
+  </si>
+  <si>
+    <t>Comparison to baseline. Example of difference is annual home load is an absolute metric (no comparison) while annual load reduction from an upgrade is a comparison metric (is old home load minus new home load)</t>
+  </si>
+  <si>
+    <t>Used to identify case (includes system sizing as well as case name and baseline type)</t>
+  </si>
+  <si>
+    <t>Not actual costs but instead internal REopt values for optimization. Important for internal understanding of process but not valuable for external facing values</t>
+  </si>
+  <si>
+    <t>Technical metrics useful for understanding results, but low priority for external facing values</t>
+  </si>
+  <si>
+    <t>Metrics which may be useful to present in some cases. In many cases these metrics are secondary or supporting metrics to other results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useful metrics which can be included in external facing values. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metrics external audience would most likely want to see. Provides good overview of what various stakeholders care about. Metrics to highlight. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -494,8 +547,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,41 +864,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416434FB-6E95-42A0-8E87-5867A3D6BEB7}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -852,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A1B421-E86A-4EC5-81CE-0CFA8BDFE657}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="A35:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,7 +2079,7 @@
         <v>131</v>
       </c>
       <c r="F53" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>